<commit_message>
check for duplicates for month in account adjust cash through monthly balance table check for unused patterns
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="balance_monthly" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="249">
   <si>
     <t xml:space="preserve">Account</t>
   </si>
@@ -48,12 +48,18 @@
     <t xml:space="preserve">Day</t>
   </si>
   <si>
+    <t xml:space="preserve">Duplicates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unicredit.Checking</t>
   </si>
   <si>
-    <t xml:space="preserve">HUF</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unicredit.Savings1</t>
   </si>
   <si>
@@ -81,9 +87,6 @@
     <t xml:space="preserve">Note</t>
   </si>
   <si>
-    <t xml:space="preserve">We don't know!!!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vouchers</t>
   </si>
   <si>
@@ -351,9 +354,6 @@
     <t xml:space="preserve">Current assets</t>
   </si>
   <si>
-    <t xml:space="preserve">Cash</t>
-  </si>
-  <si>
     <t xml:space="preserve">53.Savings</t>
   </si>
   <si>
@@ -757,9 +757,6 @@
   </si>
   <si>
     <t xml:space="preserve">Jogcím</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duplicates</t>
   </si>
   <si>
     <t xml:space="preserve">Skip</t>
@@ -862,12 +859,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -888,10 +889,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -924,162 +925,168 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="s">
+    </row>
+    <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1363491.24</v>
+      <c r="B2" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>73059</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>50000.01</v>
+        <v>1363491.24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>400013.74</v>
+        <v>50000.01</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2041912.17</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>43319.4</v>
+        <v>400013.74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.18</v>
+        <v>2041912.17</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>43319.4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.74</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>-1063</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>-1063</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>63873</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>63873</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2178.66</v>
@@ -1090,13 +1097,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1687.34</v>
@@ -1121,10 +1128,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1137,35 +1144,32 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>-73059</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -1173,10 +1177,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -1184,10 +1188,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -1195,10 +1199,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -1206,21 +1210,21 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>3</v>
@@ -1228,54 +1232,54 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>3</v>
@@ -1283,68 +1287,68 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
@@ -1352,10 +1356,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
@@ -1363,96 +1367,99 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
@@ -1461,120 +1468,114 @@
         <v>0</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B29" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C29" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>1</v>
@@ -1582,49 +1583,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1659,12 +1624,12 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>280</v>
@@ -1672,7 +1637,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>260</v>
@@ -1680,7 +1645,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -1718,604 +1683,604 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>4</v>
@@ -2323,68 +2288,68 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2422,33 +2387,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>19310</v>
@@ -2462,13 +2427,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>504226.59</v>
@@ -2482,13 +2447,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.41</v>
@@ -2502,13 +2467,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>375013.74</v>
@@ -2522,13 +2487,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>131470</v>
@@ -2542,13 +2507,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>76048</v>
@@ -2562,10 +2527,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>108</v>
@@ -2582,13 +2547,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0</v>
@@ -2602,13 +2567,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>109</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0</v>
@@ -2622,13 +2587,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>109</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>126189.64</v>
@@ -2642,13 +2607,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>60000</v>
@@ -2662,13 +2627,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>109</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>92650</v>
@@ -2708,7 +2673,7 @@
         <v>111</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
@@ -2728,7 +2693,7 @@
         <v>113</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0</v>
@@ -2748,7 +2713,7 @@
         <v>113</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
@@ -2776,10 +2741,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2792,14 +2757,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -2811,7 +2777,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>115</v>
@@ -2819,7 +2785,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>116</v>
@@ -2827,7 +2793,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>117</v>
@@ -2835,7 +2801,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>118</v>
@@ -2843,7 +2809,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>119</v>
@@ -2851,7 +2817,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>120</v>
@@ -2859,7 +2825,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>121</v>
@@ -2867,7 +2833,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>122</v>
@@ -2875,7 +2841,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>123</v>
@@ -2883,7 +2849,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>124</v>
@@ -2891,7 +2857,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>125</v>
@@ -2899,15 +2865,15 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>126</v>
@@ -2915,7 +2881,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>127</v>
@@ -2923,7 +2889,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>128</v>
@@ -2931,7 +2897,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>129</v>
@@ -2939,7 +2905,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>130</v>
@@ -2947,7 +2913,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>131</v>
@@ -2955,7 +2921,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>132</v>
@@ -2963,7 +2929,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>133</v>
@@ -2971,7 +2937,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>134</v>
@@ -3059,7 +3025,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>146</v>
@@ -3067,7 +3033,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>147</v>
@@ -3075,7 +3041,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>148</v>
@@ -3083,7 +3049,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>149</v>
@@ -3091,7 +3057,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>150</v>
@@ -3099,7 +3065,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>151</v>
@@ -3107,7 +3073,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>152</v>
@@ -3115,7 +3081,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>153</v>
@@ -3123,7 +3089,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>154</v>
@@ -3131,7 +3097,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>155</v>
@@ -3139,7 +3105,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>156</v>
@@ -3155,7 +3121,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>8430874429</v>
@@ -3163,7 +3129,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>159</v>
@@ -3171,7 +3137,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>160</v>
@@ -3179,7 +3145,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>161</v>
@@ -3187,7 +3153,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>162</v>
@@ -3195,7 +3161,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>163</v>
@@ -3203,7 +3169,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>164</v>
@@ -3211,7 +3177,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>165</v>
@@ -3219,7 +3185,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>166</v>
@@ -3230,7 +3196,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>168</v>
@@ -3241,7 +3207,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>169</v>
@@ -3249,7 +3215,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>170</v>
@@ -3257,7 +3223,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>171</v>
@@ -3265,7 +3231,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>172</v>
@@ -3273,7 +3239,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>173</v>
@@ -3281,7 +3247,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>174</v>
@@ -3292,7 +3258,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>176</v>
@@ -3300,7 +3266,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>177</v>
@@ -3308,7 +3274,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>178</v>
@@ -3316,7 +3282,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>179</v>
@@ -3324,7 +3290,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>180</v>
@@ -3332,7 +3298,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>181</v>
@@ -3340,7 +3306,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>182</v>
@@ -3348,7 +3314,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>183</v>
@@ -3359,7 +3325,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>185</v>
@@ -3367,7 +3333,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>186</v>
@@ -3375,7 +3341,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>187</v>
@@ -3386,7 +3352,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>189</v>
@@ -3397,7 +3363,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>190</v>
@@ -3405,7 +3371,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>191</v>
@@ -3413,7 +3379,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>192</v>
@@ -3421,7 +3387,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>193</v>
@@ -3429,7 +3395,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>194</v>
@@ -3437,7 +3403,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>195</v>
@@ -3445,7 +3411,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>196</v>
@@ -3453,7 +3419,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>197</v>
@@ -3461,7 +3427,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>198</v>
@@ -3469,7 +3435,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>199</v>
@@ -3477,7 +3443,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>200</v>
@@ -3485,7 +3451,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>201</v>
@@ -3493,7 +3459,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>202</v>
@@ -3501,7 +3467,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>203</v>
@@ -3509,7 +3475,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>204</v>
@@ -3517,7 +3483,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>205</v>
@@ -3525,7 +3491,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>206</v>
@@ -3533,7 +3499,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>207</v>
@@ -3572,7 +3538,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>208</v>
@@ -3603,13 +3569,13 @@
         <v>211</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>215</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3623,7 +3589,7 @@
         <v>216</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3693,7 +3659,7 @@
         <v>225</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3735,7 +3701,7 @@
         <v>229</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3749,7 +3715,7 @@
         <v>230</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3763,7 +3729,7 @@
         <v>231</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3847,7 +3813,7 @@
         <v>242</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3877,7 +3843,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
@@ -3885,22 +3851,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3908,7 +3874,7 @@
         <v>221</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>3</v>
@@ -3921,7 +3887,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -3932,27 +3898,27 @@
         <v>232</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>247</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3960,7 +3926,7 @@
         <v>217</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>112</v>
@@ -3984,7 +3950,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3998,10 +3964,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -4009,24 +3975,24 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2573.2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>